<commit_message>
Added E46 M3 definitions
</commit_message>
<xml_diff>
--- a/documents/useful/temperature sensor converter.xlsx
+++ b/documents/useful/temperature sensor converter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sorek\Documents\PlatformIO\Projects\gauge.s-sorek.uk\documents\useful\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9460871D-2159-4629-9026-C54BD97DD78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFD7D10-0468-4ABA-8A8E-5760EEBB888E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B7E37433-98C9-4AC7-A732-162F4F4FFF98}"/>
+    <workbookView xWindow="51480" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="4" xr2:uid="{B7E37433-98C9-4AC7-A732-162F4F4FFF98}"/>
   </bookViews>
   <sheets>
     <sheet name="Bosch 0261230340 oil + press" sheetId="12" r:id="rId1"/>
@@ -8463,8 +8463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A073A11A-77BF-49D7-89C7-360306EC7745}">
   <dimension ref="A1:AD46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9751,7 +9751,7 @@
   <dimension ref="A1:AD46"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10978,7 +10978,7 @@
   <dimension ref="A1:AD47"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12266,7 +12266,7 @@
   <dimension ref="A1:AD73"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X23" sqref="X23"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15149,8 +15149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9E78ED0-64E0-4567-9D45-58470B79DF18}">
   <dimension ref="A1:AD67"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17667,8 +17667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{080E139F-BBA8-45E6-8ABD-24B09CD87AA1}">
   <dimension ref="A1:AD54"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17806,7 +17806,7 @@
         <v>17.926272000000001</v>
       </c>
       <c r="D3">
-        <f t="shared" si="0"/>
+        <f>($B$2*C3)/($A$2+C3)</f>
         <v>0.42890086668912503</v>
       </c>
       <c r="E3">
@@ -18131,7 +18131,7 @@
         <v>53.875792000000004</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
+        <f>($B$2*C8)/($A$2+C8)</f>
         <v>1.0225121712170262</v>
       </c>
       <c r="E8">
@@ -18387,7 +18387,7 @@
         <v>79.151232817838547</v>
       </c>
       <c r="F12">
-        <f t="shared" si="2"/>
+        <f>($B$2*E12)/($B$6+E12)</f>
         <v>1.3115613928324668</v>
       </c>
       <c r="G12">

</xml_diff>

<commit_message>
Changed discord link, fixed few definitions, updated sensors
</commit_message>
<xml_diff>
--- a/documents/useful/temperature sensor converter.xlsx
+++ b/documents/useful/temperature sensor converter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sorek\Documents\PlatformIO\Projects\gauge.s-sorek.uk\documents\useful\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C88C3E38-E314-430F-82C0-373DEC052414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C774F03-2AEE-4A3F-82D9-8C968659F5BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29880" yWindow="0" windowWidth="21720" windowHeight="21000" xr2:uid="{B7E37433-98C9-4AC7-A732-162F4F4FFF98}"/>
+    <workbookView xWindow="51480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B7E37433-98C9-4AC7-A732-162F4F4FFF98}"/>
   </bookViews>
   <sheets>
     <sheet name="Bosch 0261230340 oil + press" sheetId="12" r:id="rId1"/>
@@ -8476,7 +8476,7 @@
   <dimension ref="A1:AD46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8620,7 +8620,7 @@
         <v>86.370583868291192</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F20" si="2">(($B$2*E3)/($B$6+E3))*$A$6/($A$6+$A$7)</f>
+        <f>(($B$2*E3)/($B$6+E3))*$A$6/($A$6+$A$7)</f>
         <v>0.18037423422626703</v>
       </c>
       <c r="G3">
@@ -8631,7 +8631,7 @@
         <v>8</v>
       </c>
       <c r="T3" s="4">
-        <f t="shared" ref="T3:T20" si="3">D3</f>
+        <f t="shared" ref="T3:T20" si="2">D3</f>
         <v>6.1936574876302226E-2</v>
       </c>
       <c r="U3" s="2" t="s">
@@ -8641,7 +8641,7 @@
         <v>9</v>
       </c>
       <c r="W3" s="3">
-        <f t="shared" ref="W3:W20" si="4">G3</f>
+        <f t="shared" ref="W3:W20" si="3">G3</f>
         <v>130</v>
       </c>
       <c r="X3" s="2" t="s">
@@ -8651,7 +8651,7 @@
         <v>8</v>
       </c>
       <c r="Z3" s="4">
-        <f t="shared" ref="Z3:Z20" si="5">F3</f>
+        <f t="shared" ref="Z3:Z20" si="4">F3</f>
         <v>0.18037423422626703</v>
       </c>
       <c r="AA3" s="2" t="s">
@@ -8661,7 +8661,7 @@
         <v>9</v>
       </c>
       <c r="AC3" s="3">
-        <f t="shared" ref="AC3:AC20" si="6">G3</f>
+        <f t="shared" ref="AC3:AC20" si="5">G3</f>
         <v>130</v>
       </c>
       <c r="AD3" s="2" t="s">
@@ -8680,7 +8680,7 @@
         <v>7.7678515779195142E-2</v>
       </c>
       <c r="E4">
-        <f t="shared" si="1"/>
+        <f>C4*$A$6/(C4+$A$6)</f>
         <v>107.75083214455539</v>
       </c>
       <c r="F4">
@@ -8695,37 +8695,37 @@
         <v>8</v>
       </c>
       <c r="T4" s="4">
+        <f t="shared" si="2"/>
+        <v>7.7678515779195142E-2</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="W4" s="3">
         <f t="shared" si="3"/>
-        <v>7.7678515779195142E-2</v>
-      </c>
-      <c r="U4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="W4" s="3">
+        <v>120</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z4" s="4">
         <f t="shared" si="4"/>
-        <v>120</v>
-      </c>
-      <c r="X4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z4" s="4">
+        <v>0.22068112551510985</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC4" s="3">
         <f t="shared" si="5"/>
-        <v>0.22068112551510985</v>
-      </c>
-      <c r="AA4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC4" s="3">
-        <f t="shared" si="6"/>
         <v>120</v>
       </c>
       <c r="AD4" s="2" t="s">
@@ -8751,7 +8751,7 @@
         <v>135.59394327148647</v>
       </c>
       <c r="F5">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="F3:F20" si="6">(($B$2*E5)/($B$6+E5))*$A$6/($A$6+$A$7)</f>
         <v>0.27089679424579322</v>
       </c>
       <c r="G5">
@@ -8762,37 +8762,37 @@
         <v>8</v>
       </c>
       <c r="T5" s="4">
+        <f t="shared" si="2"/>
+        <v>9.8431210651253986E-2</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="W5" s="3">
         <f t="shared" si="3"/>
-        <v>9.8431210651253986E-2</v>
-      </c>
-      <c r="U5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="V5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="W5" s="3">
+        <v>110</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z5" s="4">
         <f t="shared" si="4"/>
-        <v>110</v>
-      </c>
-      <c r="X5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z5" s="4">
+        <v>0.27089679424579322</v>
+      </c>
+      <c r="AA5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC5" s="3">
         <f t="shared" si="5"/>
-        <v>0.27089679424579322</v>
-      </c>
-      <c r="AA5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC5" s="3">
-        <f t="shared" si="6"/>
         <v>110</v>
       </c>
       <c r="AD5" s="2" t="s">
@@ -8818,7 +8818,7 @@
         <v>172.01039135171374</v>
       </c>
       <c r="F6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.33297364789497769</v>
       </c>
       <c r="G6">
@@ -8829,37 +8829,37 @@
         <v>8</v>
       </c>
       <c r="T6" s="4">
+        <f t="shared" si="2"/>
+        <v>0.12601399746244832</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="W6" s="3">
         <f t="shared" si="3"/>
-        <v>0.12601399746244832</v>
-      </c>
-      <c r="U6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="V6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="W6" s="3">
+        <v>100</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z6" s="4">
         <f t="shared" si="4"/>
-        <v>100</v>
-      </c>
-      <c r="X6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z6" s="4">
+        <v>0.33297364789497769</v>
+      </c>
+      <c r="AA6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC6" s="3">
         <f t="shared" si="5"/>
-        <v>0.33297364789497769</v>
-      </c>
-      <c r="AA6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC6" s="3">
-        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="AD6" s="2" t="s">
@@ -8882,7 +8882,7 @@
         <v>219.63993453355155</v>
       </c>
       <c r="F7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.40856984702093402</v>
       </c>
       <c r="G7">
@@ -8893,37 +8893,37 @@
         <v>8</v>
       </c>
       <c r="T7" s="4">
+        <f t="shared" si="2"/>
+        <v>0.16286407766990291</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="W7" s="3">
         <f t="shared" si="3"/>
-        <v>0.16286407766990291</v>
-      </c>
-      <c r="U7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="V7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="W7" s="3">
+        <v>90</v>
+      </c>
+      <c r="X7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z7" s="4">
         <f t="shared" si="4"/>
-        <v>90</v>
-      </c>
-      <c r="X7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z7" s="4">
+        <v>0.40856984702093402</v>
+      </c>
+      <c r="AA7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC7" s="3">
         <f t="shared" si="5"/>
-        <v>0.40856984702093402</v>
-      </c>
-      <c r="AA7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC7" s="3">
-        <f t="shared" si="6"/>
         <v>90</v>
       </c>
       <c r="AD7" s="2" t="s">
@@ -8943,7 +8943,7 @@
         <v>281.95292066259805</v>
       </c>
       <c r="F8">
-        <f t="shared" si="2"/>
+        <f>(($B$2*E8)/($B$6+E8))*$A$6/($A$6+$A$7)</f>
         <v>0.49898922062023926</v>
       </c>
       <c r="G8">
@@ -8954,37 +8954,37 @@
         <v>8</v>
       </c>
       <c r="T8" s="4">
+        <f t="shared" si="2"/>
+        <v>0.21244973523908109</v>
+      </c>
+      <c r="U8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="W8" s="3">
         <f t="shared" si="3"/>
-        <v>0.21244973523908109</v>
-      </c>
-      <c r="U8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="V8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="W8" s="3">
+        <v>80</v>
+      </c>
+      <c r="X8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z8" s="4">
         <f t="shared" si="4"/>
-        <v>80</v>
-      </c>
-      <c r="X8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z8" s="4">
+        <v>0.49898922062023926</v>
+      </c>
+      <c r="AA8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC8" s="3">
         <f t="shared" si="5"/>
-        <v>0.49898922062023926</v>
-      </c>
-      <c r="AA8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC8" s="3">
-        <f t="shared" si="6"/>
         <v>80</v>
       </c>
       <c r="AD8" s="2" t="s">
@@ -9004,7 +9004,7 @@
         <v>363.11814490113477</v>
       </c>
       <c r="F9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.60436748958704567</v>
       </c>
       <c r="G9">
@@ -9015,37 +9015,37 @@
         <v>8</v>
       </c>
       <c r="T9" s="4">
+        <f t="shared" si="2"/>
+        <v>0.27949327153401232</v>
+      </c>
+      <c r="U9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="W9" s="3">
         <f t="shared" si="3"/>
-        <v>0.27949327153401232</v>
-      </c>
-      <c r="U9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="V9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="W9" s="3">
+        <v>70</v>
+      </c>
+      <c r="X9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z9" s="4">
         <f t="shared" si="4"/>
-        <v>70</v>
-      </c>
-      <c r="X9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z9" s="4">
+        <v>0.60436748958704567</v>
+      </c>
+      <c r="AA9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC9" s="3">
         <f t="shared" si="5"/>
-        <v>0.60436748958704567</v>
-      </c>
-      <c r="AA9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC9" s="3">
-        <f t="shared" si="6"/>
         <v>70</v>
       </c>
       <c r="AD9" s="2" t="s">
@@ -9065,7 +9065,7 @@
         <v>467.71653543307087</v>
       </c>
       <c r="F10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.72298149141630885</v>
       </c>
       <c r="G10">
@@ -9076,37 +9076,37 @@
         <v>8</v>
       </c>
       <c r="T10" s="4">
+        <f t="shared" si="2"/>
+        <v>0.37026822818284849</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="W10" s="3">
         <f t="shared" si="3"/>
-        <v>0.37026822818284849</v>
-      </c>
-      <c r="U10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="V10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="W10" s="3">
+        <v>60</v>
+      </c>
+      <c r="X10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z10" s="4">
         <f t="shared" si="4"/>
-        <v>60</v>
-      </c>
-      <c r="X10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z10" s="4">
+        <v>0.72298149141630885</v>
+      </c>
+      <c r="AA10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC10" s="3">
         <f t="shared" si="5"/>
-        <v>0.72298149141630885</v>
-      </c>
-      <c r="AA10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC10" s="3">
-        <f t="shared" si="6"/>
         <v>60</v>
       </c>
       <c r="AD10" s="2" t="s">
@@ -9126,7 +9126,7 @@
         <v>599.47089947089944</v>
       </c>
       <c r="F11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.85031218987760493</v>
       </c>
       <c r="G11">
@@ -9137,37 +9137,37 @@
         <v>8</v>
       </c>
       <c r="T11" s="4">
+        <f t="shared" si="2"/>
+        <v>0.49225199131064445</v>
+      </c>
+      <c r="U11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="W11" s="3">
         <f t="shared" si="3"/>
-        <v>0.49225199131064445</v>
-      </c>
-      <c r="U11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="V11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="W11" s="3">
+        <v>50</v>
+      </c>
+      <c r="X11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z11" s="4">
         <f t="shared" si="4"/>
-        <v>50</v>
-      </c>
-      <c r="X11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z11" s="4">
+        <v>0.85031218987760493</v>
+      </c>
+      <c r="AA11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC11" s="3">
         <f t="shared" si="5"/>
-        <v>0.85031218987760493</v>
-      </c>
-      <c r="AA11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC11" s="3">
-        <f t="shared" si="6"/>
         <v>50</v>
       </c>
       <c r="AD11" s="2" t="s">
@@ -9187,7 +9187,7 @@
         <v>762.51856251856248</v>
       </c>
       <c r="F12">
-        <f t="shared" si="2"/>
+        <f>(($B$2*E12)/($B$6+E12))*$A$6/($A$6+$A$7)</f>
         <v>0.98152951435696933</v>
       </c>
       <c r="G12">
@@ -9198,37 +9198,37 @@
         <v>8</v>
       </c>
       <c r="T12" s="4">
+        <f t="shared" si="2"/>
+        <v>0.6564002045338333</v>
+      </c>
+      <c r="U12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="W12" s="3">
         <f t="shared" si="3"/>
-        <v>0.6564002045338333</v>
-      </c>
-      <c r="U12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="V12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="W12" s="3">
+        <v>40</v>
+      </c>
+      <c r="X12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z12" s="4">
         <f t="shared" si="4"/>
-        <v>40</v>
-      </c>
-      <c r="X12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z12" s="4">
+        <v>0.98152951435696933</v>
+      </c>
+      <c r="AA12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC12" s="3">
         <f t="shared" si="5"/>
-        <v>0.98152951435696933</v>
-      </c>
-      <c r="AA12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC12" s="3">
-        <f t="shared" si="6"/>
         <v>40</v>
       </c>
       <c r="AD12" s="2" t="s">
@@ -9248,7 +9248,7 @@
         <v>953.5410764872521</v>
       </c>
       <c r="F13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1.1073974042923433</v>
       </c>
       <c r="G13">
@@ -9259,37 +9259,37 @@
         <v>8</v>
       </c>
       <c r="T13" s="4">
+        <f t="shared" si="2"/>
+        <v>0.87010809963966784</v>
+      </c>
+      <c r="U13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="W13" s="3">
         <f t="shared" si="3"/>
-        <v>0.87010809963966784</v>
-      </c>
-      <c r="U13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="V13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="W13" s="3">
+        <v>30</v>
+      </c>
+      <c r="X13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z13" s="4">
         <f t="shared" si="4"/>
-        <v>30</v>
-      </c>
-      <c r="X13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z13" s="4">
+        <v>1.1073974042923433</v>
+      </c>
+      <c r="AA13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC13" s="3">
         <f t="shared" si="5"/>
-        <v>1.1073974042923433</v>
-      </c>
-      <c r="AA13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC13" s="3">
-        <f t="shared" si="6"/>
         <v>30</v>
       </c>
       <c r="AD13" s="2" t="s">
@@ -9309,7 +9309,7 @@
         <v>1165.8119658119658</v>
       </c>
       <c r="F14">
-        <f t="shared" si="2"/>
+        <f>(($B$2*E14)/($B$6+E14))*$A$6/($A$6+$A$7)</f>
         <v>1.2212213891081294</v>
       </c>
       <c r="G14">
@@ -9320,37 +9320,37 @@
         <v>8</v>
       </c>
       <c r="T14" s="4">
+        <f t="shared" si="2"/>
+        <v>1.13983286908078</v>
+      </c>
+      <c r="U14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="W14" s="3">
         <f t="shared" si="3"/>
-        <v>1.13983286908078</v>
-      </c>
-      <c r="U14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="V14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="W14" s="3">
+        <v>20</v>
+      </c>
+      <c r="X14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z14" s="4">
         <f t="shared" si="4"/>
-        <v>20</v>
-      </c>
-      <c r="X14" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z14" s="4">
+        <v>1.2212213891081294</v>
+      </c>
+      <c r="AA14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC14" s="3">
         <f t="shared" si="5"/>
-        <v>1.2212213891081294</v>
-      </c>
-      <c r="AA14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC14" s="3">
-        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="AD14" s="2" t="s">
@@ -9370,7 +9370,7 @@
         <v>1385.1851851851852</v>
       </c>
       <c r="F15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1.3175659937888198</v>
       </c>
       <c r="G15">
@@ -9381,37 +9381,37 @@
         <v>8</v>
       </c>
       <c r="T15" s="4">
+        <f t="shared" si="2"/>
+        <v>1.4623222748815166</v>
+      </c>
+      <c r="U15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="W15" s="3">
         <f t="shared" si="3"/>
-        <v>1.4623222748815166</v>
-      </c>
-      <c r="U15" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="V15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="W15" s="3">
+        <v>10</v>
+      </c>
+      <c r="X15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z15" s="4">
         <f t="shared" si="4"/>
-        <v>10</v>
-      </c>
-      <c r="X15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z15" s="4">
+        <v>1.3175659937888198</v>
+      </c>
+      <c r="AA15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC15" s="3">
         <f t="shared" si="5"/>
-        <v>1.3175659937888198</v>
-      </c>
-      <c r="AA15" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC15" s="3">
-        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="AD15" s="2" t="s">
@@ -9431,7 +9431,7 @@
         <v>1593.7875751503007</v>
       </c>
       <c r="F16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1.3940638762265316</v>
       </c>
       <c r="G16">
@@ -9442,37 +9442,37 @@
         <v>8</v>
       </c>
       <c r="T16" s="4">
+        <f t="shared" si="2"/>
+        <v>1.8206028233498666</v>
+      </c>
+      <c r="U16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="W16" s="3">
         <f t="shared" si="3"/>
-        <v>1.8206028233498666</v>
-      </c>
-      <c r="U16" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="V16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="W16" s="3">
+        <v>0</v>
+      </c>
+      <c r="X16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z16" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="X16" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y16" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z16" s="4">
+        <v>1.3940638762265316</v>
+      </c>
+      <c r="AA16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC16" s="3">
         <f t="shared" si="5"/>
-        <v>1.3940638762265316</v>
-      </c>
-      <c r="AA16" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC16" s="3">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AD16" s="2" t="s">
@@ -9492,7 +9492,7 @@
         <v>1775.2523036419482</v>
       </c>
       <c r="F17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1.4512567591070076</v>
       </c>
       <c r="G17">
@@ -9503,37 +9503,37 @@
         <v>8</v>
       </c>
       <c r="T17" s="4">
+        <f t="shared" si="2"/>
+        <v>2.1837711406980929</v>
+      </c>
+      <c r="U17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="W17" s="3">
         <f t="shared" si="3"/>
-        <v>2.1837711406980929</v>
-      </c>
-      <c r="U17" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="V17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="W17" s="3">
+        <v>-10</v>
+      </c>
+      <c r="X17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z17" s="4">
         <f t="shared" si="4"/>
-        <v>-10</v>
-      </c>
-      <c r="X17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z17" s="4">
+        <v>1.4512567591070076</v>
+      </c>
+      <c r="AA17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC17" s="3">
         <f t="shared" si="5"/>
-        <v>1.4512567591070076</v>
-      </c>
-      <c r="AA17" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC17" s="3">
-        <f t="shared" si="6"/>
         <v>-10</v>
       </c>
       <c r="AD17" s="2" t="s">
@@ -9553,7 +9553,7 @@
         <v>1919.696530955001</v>
       </c>
       <c r="F18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1.4917000648624201</v>
       </c>
       <c r="G18">
@@ -9564,37 +9564,37 @@
         <v>8</v>
       </c>
       <c r="T18" s="4">
+        <f t="shared" si="2"/>
+        <v>2.5153589315525875</v>
+      </c>
+      <c r="U18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="W18" s="3">
         <f t="shared" si="3"/>
-        <v>2.5153589315525875</v>
-      </c>
-      <c r="U18" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="V18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="W18" s="3">
+        <v>-20</v>
+      </c>
+      <c r="X18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z18" s="4">
         <f t="shared" si="4"/>
-        <v>-20</v>
-      </c>
-      <c r="X18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z18" s="4">
+        <v>1.4917000648624201</v>
+      </c>
+      <c r="AA18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC18" s="3">
         <f t="shared" si="5"/>
-        <v>1.4917000648624201</v>
-      </c>
-      <c r="AA18" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC18" s="3">
-        <f t="shared" si="6"/>
         <v>-20</v>
       </c>
       <c r="AD18" s="2" t="s">
@@ -9614,7 +9614,7 @@
         <v>2025.4220170249603</v>
       </c>
       <c r="F19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1.5188546177250442</v>
       </c>
       <c r="G19">
@@ -9625,37 +9625,37 @@
         <v>8</v>
       </c>
       <c r="T19" s="4">
+        <f t="shared" si="2"/>
+        <v>2.7868316569613549</v>
+      </c>
+      <c r="U19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="W19" s="3">
         <f t="shared" si="3"/>
-        <v>2.7868316569613549</v>
-      </c>
-      <c r="U19" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="V19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="W19" s="3">
+        <v>-30</v>
+      </c>
+      <c r="X19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z19" s="4">
         <f t="shared" si="4"/>
-        <v>-30</v>
-      </c>
-      <c r="X19" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z19" s="4">
+        <v>1.5188546177250442</v>
+      </c>
+      <c r="AA19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC19" s="3">
         <f t="shared" si="5"/>
-        <v>1.5188546177250442</v>
-      </c>
-      <c r="AA19" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC19" s="3">
-        <f t="shared" si="6"/>
         <v>-30</v>
       </c>
       <c r="AD19" s="2" t="s">
@@ -9675,7 +9675,7 @@
         <v>2097.1613122556519</v>
       </c>
       <c r="F20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1.5362243833902287</v>
       </c>
       <c r="G20">
@@ -9686,17 +9686,17 @@
         <v>8</v>
       </c>
       <c r="T20" s="4">
+        <f t="shared" si="2"/>
+        <v>2.9870712613994024</v>
+      </c>
+      <c r="U20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="W20" s="3">
         <f t="shared" si="3"/>
-        <v>2.9870712613994024</v>
-      </c>
-      <c r="U20" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="V20" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="W20" s="3">
-        <f t="shared" si="4"/>
         <v>-40</v>
       </c>
       <c r="X20" s="2" t="s">
@@ -9706,17 +9706,17 @@
         <v>8</v>
       </c>
       <c r="Z20" s="4">
+        <f t="shared" si="4"/>
+        <v>1.5362243833902287</v>
+      </c>
+      <c r="AA20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC20" s="3">
         <f t="shared" si="5"/>
-        <v>1.5362243833902287</v>
-      </c>
-      <c r="AA20" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB20" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC20" s="3">
-        <f t="shared" si="6"/>
         <v>-40</v>
       </c>
       <c r="AD20" s="2" t="s">
@@ -9766,7 +9766,7 @@
   <dimension ref="A1:AD46"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10355,7 +10355,7 @@
         <v>661.57659890927118</v>
       </c>
       <c r="F10">
-        <f t="shared" si="1"/>
+        <f>(($B$2*E10)/($B$6+E10))*$A$6/($A$6+$A$7)</f>
         <v>0.90332995166199215</v>
       </c>
       <c r="G10">
@@ -10416,7 +10416,7 @@
         <v>859.42857142857144</v>
       </c>
       <c r="F11">
-        <f t="shared" si="1"/>
+        <f>(($B$2*E11)/($B$6+E11))*$A$6/($A$6+$A$7)</f>
         <v>1.048617086662569</v>
       </c>
       <c r="G11">

</xml_diff>

<commit_message>
Updated configs to match v2.0; new view of file editor + updates; gauge.html to handle remote gauge control
</commit_message>
<xml_diff>
--- a/documents/useful/temperature sensor converter.xlsx
+++ b/documents/useful/temperature sensor converter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sorek\Documents\PlatformIO\Projects\gauge.s-sorek.uk\documents\useful\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Programming\gauge.s-sorek.uk\documents\useful\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56ACFB3E-9C90-45CD-B206-9769DF207CEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DCB0AA5-BFBE-44D0-9DAC-B8567FF76F12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29880" yWindow="0" windowWidth="21720" windowHeight="21000" firstSheet="6" activeTab="7" xr2:uid="{B7E37433-98C9-4AC7-A732-162F4F4FFF98}"/>
+    <workbookView xWindow="30165" yWindow="-15" windowWidth="21555" windowHeight="21015" xr2:uid="{B7E37433-98C9-4AC7-A732-162F4F4FFF98}"/>
   </bookViews>
   <sheets>
     <sheet name="Bosch 0261230340 oil + press" sheetId="12" r:id="rId1"/>
@@ -229,7 +229,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -320,7 +320,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="pl-PL"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -530,7 +530,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="pl-PL"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -542,61 +542,61 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>0.14905681928509013</c:v>
+                  <c:v>0.27491469383262346</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.18243449482611149</c:v>
+                  <c:v>0.33206022399058982</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.22377294020991007</c:v>
+                  <c:v>0.4007897315409753</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.27557067430192544</c:v>
+                  <c:v>0.48386717371701882</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.34006305664052694</c:v>
+                  <c:v>0.58285254052212165</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.41929558795682637</c:v>
+                  <c:v>0.69817597073985904</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.51508112709179765</c:v>
+                  <c:v>0.82910953897395789</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.62813563098568015</c:v>
+                  <c:v>0.97285300567343058</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.75725925405633188</c:v>
+                  <c:v>1.1242784964570069</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.89812635118904627</c:v>
+                  <c:v>1.2757920597819594</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.0457970227368107</c:v>
+                  <c:v>1.4211726105707054</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.1898973569912157</c:v>
+                  <c:v>1.5513825033995983</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.3223266745005873</c:v>
+                  <c:v>1.6620633631194153</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.4360270784852969</c:v>
+                  <c:v>1.7509318131988596</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.527375894779724</c:v>
+                  <c:v>1.8185654446996704</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.5963007245510414</c:v>
+                  <c:v>1.8675299933278222</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.6453687798391732</c:v>
+                  <c:v>1.9013616586798987</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.6784682719690438</c:v>
+                  <c:v>1.9237190691115296</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.6997060984570167</c:v>
+                  <c:v>1.9378724473671181</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -740,7 +740,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="789408384"/>
@@ -802,7 +802,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="646701888"/>
@@ -843,7 +843,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pl-PL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -857,7 +857,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -948,7 +948,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="pl-PL"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1155,7 +1155,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="pl-PL"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1359,7 +1359,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="789408384"/>
@@ -1421,7 +1421,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="646701888"/>
@@ -1462,7 +1462,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pl-PL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1476,7 +1476,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1567,7 +1567,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="pl-PL"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1780,7 +1780,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="pl-PL"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1990,7 +1990,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="789408384"/>
@@ -2052,7 +2052,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="646701888"/>
@@ -2093,7 +2093,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pl-PL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2107,7 +2107,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2197,7 +2197,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="pl-PL"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2563,7 +2563,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="pl-PL"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2929,7 +2929,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="789408384"/>
@@ -2991,7 +2991,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="646701888"/>
@@ -3032,7 +3032,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pl-PL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3046,7 +3046,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3136,7 +3136,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="pl-PL"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3463,7 +3463,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="pl-PL"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3793,7 +3793,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="789408384"/>
@@ -3855,7 +3855,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="646701888"/>
@@ -3896,7 +3896,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pl-PL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3910,7 +3910,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4001,7 +4001,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="pl-PL"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -4256,7 +4256,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="pl-PL"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -4508,7 +4508,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="789408384"/>
@@ -4570,7 +4570,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="646701888"/>
@@ -4611,7 +4611,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pl-PL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4625,7 +4625,7 @@
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4716,7 +4716,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="pl-PL"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -4902,7 +4902,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="pl-PL"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -5088,7 +5088,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="789408384"/>
@@ -5150,7 +5150,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="646701888"/>
@@ -5191,7 +5191,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pl-PL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5205,7 +5205,7 @@
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5296,7 +5296,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="pl-PL"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -5488,7 +5488,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="pl-PL"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -5680,7 +5680,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="789408384"/>
@@ -5742,7 +5742,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="646701888"/>
@@ -5783,7 +5783,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pl-PL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -10883,8 +10883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A073A11A-77BF-49D7-89C7-360306EC7745}">
   <dimension ref="A1:AD46"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10969,7 +10969,7 @@
       </c>
       <c r="F2" s="11">
         <f>(($B$2*E2)/($B$6+E2))*$A$6/($A$6+$A$7)</f>
-        <v>0.14905681928509013</v>
+        <v>0.27491469383262346</v>
       </c>
       <c r="G2" s="9">
         <v>140</v>
@@ -11000,7 +11000,7 @@
       </c>
       <c r="Z2" s="4">
         <f>F2</f>
-        <v>0.14905681928509013</v>
+        <v>0.27491469383262346</v>
       </c>
       <c r="AA2" s="2" t="s">
         <v>3</v>
@@ -11030,7 +11030,7 @@
       </c>
       <c r="F3" s="11">
         <f>(($B$2*E3)/($B$6+E3))*$A$6/($A$6+$A$7)</f>
-        <v>0.18243449482611149</v>
+        <v>0.33206022399058982</v>
       </c>
       <c r="G3" s="9">
         <v>130</v>
@@ -11061,7 +11061,7 @@
       </c>
       <c r="Z3" s="4">
         <f t="shared" ref="Z3:Z20" si="4">F3</f>
-        <v>0.18243449482611149</v>
+        <v>0.33206022399058982</v>
       </c>
       <c r="AA3" s="2" t="s">
         <v>3</v>
@@ -11094,7 +11094,7 @@
       </c>
       <c r="F4" s="11">
         <f>(($B$2*E4)/($B$6+E4))*$A$6/($A$6+$A$7)</f>
-        <v>0.22377294020991007</v>
+        <v>0.4007897315409753</v>
       </c>
       <c r="G4" s="9">
         <v>120</v>
@@ -11125,7 +11125,7 @@
       </c>
       <c r="Z4" s="4">
         <f t="shared" si="4"/>
-        <v>0.22377294020991007</v>
+        <v>0.4007897315409753</v>
       </c>
       <c r="AA4" s="2" t="s">
         <v>3</v>
@@ -11161,7 +11161,7 @@
       </c>
       <c r="F5" s="11">
         <f>(($B$2*E5)/($B$6+E5))*$A$6/($A$6+$A$7)</f>
-        <v>0.27557067430192544</v>
+        <v>0.48386717371701882</v>
       </c>
       <c r="G5" s="9">
         <v>110</v>
@@ -11192,7 +11192,7 @@
       </c>
       <c r="Z5" s="4">
         <f t="shared" si="4"/>
-        <v>0.27557067430192544</v>
+        <v>0.48386717371701882</v>
       </c>
       <c r="AA5" s="2" t="s">
         <v>3</v>
@@ -11213,7 +11213,7 @@
         <v>2200</v>
       </c>
       <c r="B6">
-        <v>1000</v>
+        <v>510</v>
       </c>
       <c r="C6" s="9">
         <v>186.6</v>
@@ -11228,7 +11228,7 @@
       </c>
       <c r="F6" s="11">
         <f t="shared" ref="F6:F20" si="6">(($B$2*E6)/($B$6+E6))*$A$6/($A$6+$A$7)</f>
-        <v>0.34006305664052694</v>
+        <v>0.58285254052212165</v>
       </c>
       <c r="G6" s="9">
         <v>100</v>
@@ -11259,7 +11259,7 @@
       </c>
       <c r="Z6" s="4">
         <f t="shared" si="4"/>
-        <v>0.34006305664052694</v>
+        <v>0.58285254052212165</v>
       </c>
       <c r="AA6" s="2" t="s">
         <v>3</v>
@@ -11292,7 +11292,7 @@
       </c>
       <c r="F7" s="11">
         <f>(($B$2*E7)/($B$6+E7))*$A$6/($A$6+$A$7)</f>
-        <v>0.41929558795682637</v>
+        <v>0.69817597073985904</v>
       </c>
       <c r="G7" s="9">
         <v>90</v>
@@ -11323,7 +11323,7 @@
       </c>
       <c r="Z7" s="4">
         <f t="shared" si="4"/>
-        <v>0.41929558795682637</v>
+        <v>0.69817597073985904</v>
       </c>
       <c r="AA7" s="2" t="s">
         <v>3</v>
@@ -11353,7 +11353,7 @@
       </c>
       <c r="F8" s="11">
         <f>(($B$2*E8)/($B$6+E8))*$A$6/($A$6+$A$7)</f>
-        <v>0.51508112709179765</v>
+        <v>0.82910953897395789</v>
       </c>
       <c r="G8" s="9">
         <v>80</v>
@@ -11384,7 +11384,7 @@
       </c>
       <c r="Z8" s="4">
         <f t="shared" si="4"/>
-        <v>0.51508112709179765</v>
+        <v>0.82910953897395789</v>
       </c>
       <c r="AA8" s="2" t="s">
         <v>3</v>
@@ -11414,7 +11414,7 @@
       </c>
       <c r="F9" s="11">
         <f t="shared" si="6"/>
-        <v>0.62813563098568015</v>
+        <v>0.97285300567343058</v>
       </c>
       <c r="G9" s="9">
         <v>70</v>
@@ -11445,7 +11445,7 @@
       </c>
       <c r="Z9" s="4">
         <f t="shared" si="4"/>
-        <v>0.62813563098568015</v>
+        <v>0.97285300567343058</v>
       </c>
       <c r="AA9" s="2" t="s">
         <v>3</v>
@@ -11475,7 +11475,7 @@
       </c>
       <c r="F10" s="11">
         <f t="shared" si="6"/>
-        <v>0.75725925405633188</v>
+        <v>1.1242784964570069</v>
       </c>
       <c r="G10" s="9">
         <v>60</v>
@@ -11506,7 +11506,7 @@
       </c>
       <c r="Z10" s="4">
         <f t="shared" si="4"/>
-        <v>0.75725925405633188</v>
+        <v>1.1242784964570069</v>
       </c>
       <c r="AA10" s="2" t="s">
         <v>3</v>
@@ -11536,7 +11536,7 @@
       </c>
       <c r="F11" s="11">
         <f t="shared" si="6"/>
-        <v>0.89812635118904627</v>
+        <v>1.2757920597819594</v>
       </c>
       <c r="G11" s="9">
         <v>50</v>
@@ -11567,7 +11567,7 @@
       </c>
       <c r="Z11" s="4">
         <f t="shared" si="4"/>
-        <v>0.89812635118904627</v>
+        <v>1.2757920597819594</v>
       </c>
       <c r="AA11" s="2" t="s">
         <v>3</v>
@@ -11597,7 +11597,7 @@
       </c>
       <c r="F12" s="11">
         <f>(($B$2*E12)/($B$6+E12))*$A$6/($A$6+$A$7)</f>
-        <v>1.0457970227368107</v>
+        <v>1.4211726105707054</v>
       </c>
       <c r="G12" s="9">
         <v>40</v>
@@ -11628,7 +11628,7 @@
       </c>
       <c r="Z12" s="4">
         <f t="shared" si="4"/>
-        <v>1.0457970227368107</v>
+        <v>1.4211726105707054</v>
       </c>
       <c r="AA12" s="2" t="s">
         <v>3</v>
@@ -11658,7 +11658,7 @@
       </c>
       <c r="F13" s="11">
         <f t="shared" si="6"/>
-        <v>1.1898973569912157</v>
+        <v>1.5513825033995983</v>
       </c>
       <c r="G13" s="9">
         <v>30</v>
@@ -11689,7 +11689,7 @@
       </c>
       <c r="Z13" s="4">
         <f t="shared" si="4"/>
-        <v>1.1898973569912157</v>
+        <v>1.5513825033995983</v>
       </c>
       <c r="AA13" s="2" t="s">
         <v>3</v>
@@ -11719,7 +11719,7 @@
       </c>
       <c r="F14" s="11">
         <f>(($B$2*E14)/($B$6+E14))*$A$6/($A$6+$A$7)</f>
-        <v>1.3223266745005873</v>
+        <v>1.6620633631194153</v>
       </c>
       <c r="G14" s="9">
         <v>20</v>
@@ -11750,7 +11750,7 @@
       </c>
       <c r="Z14" s="4">
         <f t="shared" si="4"/>
-        <v>1.3223266745005873</v>
+        <v>1.6620633631194153</v>
       </c>
       <c r="AA14" s="2" t="s">
         <v>3</v>
@@ -11780,7 +11780,7 @@
       </c>
       <c r="F15" s="11">
         <f t="shared" si="6"/>
-        <v>1.4360270784852969</v>
+        <v>1.7509318131988596</v>
       </c>
       <c r="G15" s="9">
         <v>10</v>
@@ -11811,7 +11811,7 @@
       </c>
       <c r="Z15" s="4">
         <f t="shared" si="4"/>
-        <v>1.4360270784852969</v>
+        <v>1.7509318131988596</v>
       </c>
       <c r="AA15" s="2" t="s">
         <v>3</v>
@@ -11841,7 +11841,7 @@
       </c>
       <c r="F16" s="11">
         <f t="shared" si="6"/>
-        <v>1.527375894779724</v>
+        <v>1.8185654446996704</v>
       </c>
       <c r="G16" s="9">
         <v>0</v>
@@ -11872,7 +11872,7 @@
       </c>
       <c r="Z16" s="4">
         <f t="shared" si="4"/>
-        <v>1.527375894779724</v>
+        <v>1.8185654446996704</v>
       </c>
       <c r="AA16" s="2" t="s">
         <v>3</v>
@@ -11902,7 +11902,7 @@
       </c>
       <c r="F17" s="11">
         <f t="shared" si="6"/>
-        <v>1.5963007245510414</v>
+        <v>1.8675299933278222</v>
       </c>
       <c r="G17" s="9">
         <v>-10</v>
@@ -11933,7 +11933,7 @@
       </c>
       <c r="Z17" s="4">
         <f t="shared" si="4"/>
-        <v>1.5963007245510414</v>
+        <v>1.8675299933278222</v>
       </c>
       <c r="AA17" s="2" t="s">
         <v>3</v>
@@ -11963,7 +11963,7 @@
       </c>
       <c r="F18" s="11">
         <f t="shared" si="6"/>
-        <v>1.6453687798391732</v>
+        <v>1.9013616586798987</v>
       </c>
       <c r="G18" s="9">
         <v>-20</v>
@@ -11994,7 +11994,7 @@
       </c>
       <c r="Z18" s="4">
         <f t="shared" si="4"/>
-        <v>1.6453687798391732</v>
+        <v>1.9013616586798987</v>
       </c>
       <c r="AA18" s="2" t="s">
         <v>3</v>
@@ -12024,7 +12024,7 @@
       </c>
       <c r="F19" s="11">
         <f t="shared" si="6"/>
-        <v>1.6784682719690438</v>
+        <v>1.9237190691115296</v>
       </c>
       <c r="G19" s="9">
         <v>-30</v>
@@ -12055,7 +12055,7 @@
       </c>
       <c r="Z19" s="4">
         <f t="shared" si="4"/>
-        <v>1.6784682719690438</v>
+        <v>1.9237190691115296</v>
       </c>
       <c r="AA19" s="2" t="s">
         <v>3</v>
@@ -12085,7 +12085,7 @@
       </c>
       <c r="F20" s="11">
         <f t="shared" si="6"/>
-        <v>1.6997060984570167</v>
+        <v>1.9378724473671181</v>
       </c>
       <c r="G20" s="9">
         <v>-40</v>
@@ -12116,7 +12116,7 @@
       </c>
       <c r="Z20" s="4">
         <f t="shared" si="4"/>
-        <v>1.6997060984570167</v>
+        <v>1.9378724473671181</v>
       </c>
       <c r="AA20" s="2" t="s">
         <v>3</v>
@@ -23321,7 +23321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3352653-DA5C-4691-9AF3-58B474D2357C}">
   <dimension ref="A1:AD45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
@@ -24630,7 +24630,7 @@
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C30">
-        <f t="shared" ref="C26:C41" si="10">($A$26*D30)/($B$26-D30)</f>
+        <f t="shared" ref="C30:C41" si="10">($A$26*D30)/($B$26-D30)</f>
         <v>859.87192457541369</v>
       </c>
       <c r="D30">

</xml_diff>

<commit_message>
Update definitions and cleanup; added new sensors to the converter xls
</commit_message>
<xml_diff>
--- a/documents/useful/temperature sensor converter.xlsx
+++ b/documents/useful/temperature sensor converter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Programming\gauge.s-sorek.uk\documents\useful\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E6F1C9-9C57-40E4-BD17-A069C95D62F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D21709-1D4D-44B1-95DC-63C9F639A667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30165" yWindow="-15" windowWidth="21555" windowHeight="21135" firstSheet="7" activeTab="9" xr2:uid="{B7E37433-98C9-4AC7-A732-162F4F4FFF98}"/>
+    <workbookView xWindow="-120" yWindow="-15" windowWidth="30495" windowHeight="21135" firstSheet="7" activeTab="11" xr2:uid="{B7E37433-98C9-4AC7-A732-162F4F4FFF98}"/>
   </bookViews>
   <sheets>
     <sheet name="Bosch 0280130026 oil temp" sheetId="11" r:id="rId1"/>
@@ -23,18 +23,31 @@
     <sheet name="Bosch E36 coolant sensor" sheetId="16" r:id="rId8"/>
     <sheet name="VDO 360-081-029-001K pressure" sheetId="9" r:id="rId9"/>
     <sheet name="27 NPT 3-160 pressure" sheetId="18" r:id="rId10"/>
+    <sheet name="Beta (osculati)" sheetId="19" r:id="rId11"/>
+    <sheet name="Bosch E36 coolant sensor (2)" sheetId="21" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2212" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2321" uniqueCount="34">
   <si>
     <t>Voltage (V)</t>
   </si>
@@ -119,6 +132,24 @@
   <si>
     <t>https://www.prosportgauges.co.uk/shop/oil-pressure-sensor-3-160-ohms</t>
   </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>T0 (°C)</t>
+  </si>
+  <si>
+    <t>R (Ohm)</t>
+  </si>
+  <si>
+    <t>B (K)</t>
+  </si>
+  <si>
+    <t>P (Ohm)</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
 </sst>
 </file>
 
@@ -154,7 +185,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -173,8 +204,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -191,12 +234,128 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -219,6 +378,46 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -240,7 +439,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -859,7 +1058,7 @@
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1571,10 +1770,1335 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Temp sensor</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="5"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Beta (osculati)'!$A$7:$A$71</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="65"/>
+                <c:pt idx="0">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.05</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.1499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.35</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.45</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.55</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.65</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.85</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.95</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2.0499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2.15</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2.35</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2.4500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2.5499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2.65</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2.85</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2.95</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>3.05</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>3.15</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>3.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Beta (osculati)'!$B$7:$B$71</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="65"/>
+                <c:pt idx="0">
+                  <c:v>162.70570122617875</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>130.94661336106805</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>114.17146120914816</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>102.91601436410565</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>94.493723678017204</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>87.77967224545398</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>82.200422673284493</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>77.425728358465676</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>73.248759010494325</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>69.531763738385052</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>66.178569432784514</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>63.119472728013761</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60.302392856418692</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>57.687417972539663</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>55.243298385908872</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>52.945110491530329</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>50.772653009122678</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>48.709316998419069</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>46.741271433122506</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>44.856864348117483</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43.046174571623965</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>41.300670737318001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>39.612948072577126</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>37.976522456330883</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>36.385667232743458</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>34.835282336065518</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>33.320788093115539</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>31.838038042164669</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>30.383246509841058</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>28.952927697270297</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>27.543843760225059</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>26.152959904599129</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>24.777404911952431</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>23.414435797205442</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>22.061405507256666</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>20.715732712617523</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>19.374872835437941</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>18.036289503204216</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>16.69742562074714</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>15.355673213185241</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>14.008341104398937</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>12.652619350391774</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>11.285539129341487</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>9.9039264769240276</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>8.5043478113066726</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>7.0830445637105299</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>5.6358533365022367</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.1581067262493434</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2.6445080777326098</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.088970662157692</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-0.51559241654928201</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-2.1775477564728476</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>-3.9069210617709587</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-5.7159235818964476</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>-7.6197009771478861</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>-9.6374294493601838</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>-11.793974535950554</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>-14.122502737830132</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-16.668795322814162</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-19.498810814754705</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>-22.712991819120049</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>-26.476219372872094</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>-31.090168576091429</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-37.211298628077486</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>-46.839474542638158</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B70C-4FEA-9BBC-6A6FE44F7C08}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="141810944"/>
+        <c:axId val="141811904"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="141810944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="141811904"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="141811904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="141810944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Bosch E36 coolant sensor (2)'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Temperature (°C)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.5234547115180995E-2"/>
+                  <c:y val="-0.47986147066810153"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>y </a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                        <a:effectLst/>
+                      </a:rPr>
+                      <a:t>= -8.9368x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="30000">
+                        <a:effectLst/>
+                      </a:rPr>
+                      <a:t>3</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                        <a:effectLst/>
+                      </a:rPr>
+                      <a:t> + 51.392x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="30000">
+                        <a:effectLst/>
+                      </a:rPr>
+                      <a:t>2</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                        <a:effectLst/>
+                      </a:rPr>
+                      <a:t> - 143.25x + 235.45</a:t>
+                    </a:r>
+                    <a:br>
+                      <a:rPr lang="en-US" baseline="0"/>
+                    </a:br>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>R² = 1</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln w="31750">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Bosch E36 coolant sensor (2)'!$D$2:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2.8478832716810518</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.6792325056433408</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.4791044776119402</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.2550348321722606</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0154534838458544</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.7722222222222221</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5352941176470589</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.3180180180180181</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1217821782178219</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.95124555160142343</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.80566893424036268</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Bosch E36 coolant sensor (2)'!$G$2:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>37.777777777777779</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>48.888888888888886</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>71.111111111111114</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>82.222222222222229</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>93.333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>104.44444444444444</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>115.55555555555556</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>126.66666666666667</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>137.77777777777777</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>148.88888888888889</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B396-4861-B2AE-7353CC3ADF54}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="5"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.21466134090070507"/>
+                  <c:y val="-0.73754440590189851"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln w="31750">
+                  <a:solidFill>
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Bosch E36 coolant sensor (2)'!$F$2:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.5420504589321482</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4692111482051089</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3803324099722991</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2775269904432627</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1635518600992869</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0433102081268582</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.92153487014881807</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.80558985483063561</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.69716576542979669</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.5999387880024486</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.51463371812316205</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Bosch E36 coolant sensor (2)'!$G$2:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>37.777777777777779</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>48.888888888888886</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>71.111111111111114</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>82.222222222222229</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>93.333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>104.44444444444444</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>115.55555555555556</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>126.66666666666667</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>137.77777777777777</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>148.88888888888889</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-B396-4861-B2AE-7353CC3ADF54}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="646701888"/>
+        <c:axId val="789408384"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="646701888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="789408384"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="789408384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="646701888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2145,7 +3669,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2773,7 +4297,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3404,7 +4928,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4343,7 +5867,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5207,7 +6731,7 @@
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5787,7 +7311,7 @@
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -6379,7 +7903,7 @@
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -7132,6 +8656,86 @@
 </file>
 
 <file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors12.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -8523,6 +10127,1038 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -12715,6 +15351,90 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFD28F23-360C-4800-89AA-D8AEE05DD9BA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>290512</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>128586</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE0D7FE4-B19C-5CBD-4C7D-E32D012023A3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>347382</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>33618</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E408446B-F6D2-4267-8C23-17466C459213}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13080,9 +15800,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -13120,7 +15840,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -13226,7 +15946,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -13368,7 +16088,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -14613,7 +17333,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C58B430-22D6-4B3A-9457-9E587F0FF4F9}">
   <dimension ref="A1:AD54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
@@ -14779,7 +17499,7 @@
         <v>9</v>
       </c>
       <c r="W3" s="12">
-        <f t="shared" ref="W3:W27" si="4">G3</f>
+        <f t="shared" ref="W3:W25" si="4">G3</f>
         <v>0.4</v>
       </c>
       <c r="X3" s="2" t="s">
@@ -16334,6 +19054,1473 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
   <drawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DBD1E45-E85C-4EE8-A288-6CA01A4E41AE}">
+  <dimension ref="A1:D71"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="19"/>
+    <col min="3" max="4" width="9.140625" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="20">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="21">
+        <v>990.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="21">
+        <v>3930</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="21">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="22">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="B7" s="16">
+        <f t="shared" ref="B7:B38" si="0">1/(1/$B$3 * LN((($B$4*A7)/($B$5-A7))/$B$2)+1/($B$1+273.15)) - 273.15</f>
+        <v>162.70570122617875</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="B8" s="16">
+        <f t="shared" si="0"/>
+        <v>130.94661336106805</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="15">
+        <v>0.15</v>
+      </c>
+      <c r="B9" s="16">
+        <f t="shared" si="0"/>
+        <v>114.17146120914816</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="B10" s="16">
+        <f t="shared" si="0"/>
+        <v>102.91601436410565</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="B11" s="16">
+        <f t="shared" si="0"/>
+        <v>94.493723678017204</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="B12" s="16">
+        <f t="shared" si="0"/>
+        <v>87.77967224545398</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
+        <v>0.35</v>
+      </c>
+      <c r="B13" s="16">
+        <f t="shared" si="0"/>
+        <v>82.200422673284493</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="B14" s="16">
+        <f t="shared" si="0"/>
+        <v>77.425728358465676</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="15">
+        <v>0.45</v>
+      </c>
+      <c r="B15" s="16">
+        <f t="shared" si="0"/>
+        <v>73.248759010494325</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="B16" s="16">
+        <f t="shared" si="0"/>
+        <v>69.531763738385052</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="15">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="B17" s="16">
+        <f t="shared" si="0"/>
+        <v>66.178569432784514</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="15">
+        <v>0.6</v>
+      </c>
+      <c r="B18" s="16">
+        <f t="shared" si="0"/>
+        <v>63.119472728013761</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="15">
+        <v>0.65</v>
+      </c>
+      <c r="B19" s="16">
+        <f t="shared" si="0"/>
+        <v>60.302392856418692</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="15">
+        <v>0.7</v>
+      </c>
+      <c r="B20" s="16">
+        <f t="shared" si="0"/>
+        <v>57.687417972539663</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="15">
+        <v>0.75</v>
+      </c>
+      <c r="B21" s="16">
+        <f t="shared" si="0"/>
+        <v>55.243298385908872</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="B22" s="16">
+        <f t="shared" si="0"/>
+        <v>52.945110491530329</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="15">
+        <v>0.85</v>
+      </c>
+      <c r="B23" s="16">
+        <f t="shared" si="0"/>
+        <v>50.772653009122678</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="B24" s="16">
+        <f t="shared" si="0"/>
+        <v>48.709316998419069</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="15">
+        <v>0.95</v>
+      </c>
+      <c r="B25" s="16">
+        <f t="shared" si="0"/>
+        <v>46.741271433122506</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="15">
+        <v>1</v>
+      </c>
+      <c r="B26" s="16">
+        <f t="shared" si="0"/>
+        <v>44.856864348117483</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="15">
+        <v>1.05</v>
+      </c>
+      <c r="B27" s="16">
+        <f t="shared" si="0"/>
+        <v>43.046174571623965</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B28" s="16">
+        <f t="shared" si="0"/>
+        <v>41.300670737318001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="15">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="B29" s="16">
+        <f t="shared" si="0"/>
+        <v>39.612948072577126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="15">
+        <v>1.2</v>
+      </c>
+      <c r="B30" s="16">
+        <f t="shared" si="0"/>
+        <v>37.976522456330883</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="15">
+        <v>1.25</v>
+      </c>
+      <c r="B31" s="16">
+        <f t="shared" si="0"/>
+        <v>36.385667232743458</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="15">
+        <v>1.3</v>
+      </c>
+      <c r="B32" s="16">
+        <f t="shared" si="0"/>
+        <v>34.835282336065518</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="15">
+        <v>1.35</v>
+      </c>
+      <c r="B33" s="16">
+        <f t="shared" si="0"/>
+        <v>33.320788093115539</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="15">
+        <v>1.4</v>
+      </c>
+      <c r="B34" s="16">
+        <f t="shared" si="0"/>
+        <v>31.838038042164669</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="15">
+        <v>1.45</v>
+      </c>
+      <c r="B35" s="16">
+        <f t="shared" si="0"/>
+        <v>30.383246509841058</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="15">
+        <v>1.5</v>
+      </c>
+      <c r="B36" s="16">
+        <f t="shared" si="0"/>
+        <v>28.952927697270297</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="15">
+        <v>1.55</v>
+      </c>
+      <c r="B37" s="16">
+        <f t="shared" si="0"/>
+        <v>27.543843760225059</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="15">
+        <v>1.6</v>
+      </c>
+      <c r="B38" s="16">
+        <f t="shared" si="0"/>
+        <v>26.152959904599129</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="15">
+        <v>1.65</v>
+      </c>
+      <c r="B39" s="16">
+        <f t="shared" ref="B39:B70" si="1">1/(1/$B$3 * LN((($B$4*A39)/($B$5-A39))/$B$2)+1/($B$1+273.15)) - 273.15</f>
+        <v>24.777404911952431</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="15">
+        <v>1.7</v>
+      </c>
+      <c r="B40" s="16">
+        <f t="shared" si="1"/>
+        <v>23.414435797205442</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="15">
+        <v>1.75</v>
+      </c>
+      <c r="B41" s="16">
+        <f t="shared" si="1"/>
+        <v>22.061405507256666</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="15">
+        <v>1.8</v>
+      </c>
+      <c r="B42" s="16">
+        <f t="shared" si="1"/>
+        <v>20.715732712617523</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="15">
+        <v>1.85</v>
+      </c>
+      <c r="B43" s="16">
+        <f t="shared" si="1"/>
+        <v>19.374872835437941</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="15">
+        <v>1.9</v>
+      </c>
+      <c r="B44" s="16">
+        <f t="shared" si="1"/>
+        <v>18.036289503204216</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="15">
+        <v>1.95</v>
+      </c>
+      <c r="B45" s="16">
+        <f t="shared" si="1"/>
+        <v>16.69742562074714</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="15">
+        <v>2</v>
+      </c>
+      <c r="B46" s="16">
+        <f t="shared" si="1"/>
+        <v>15.355673213185241</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="15">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="B47" s="16">
+        <f t="shared" si="1"/>
+        <v>14.008341104398937</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="15">
+        <v>2.1</v>
+      </c>
+      <c r="B48" s="16">
+        <f t="shared" si="1"/>
+        <v>12.652619350391774</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="15">
+        <v>2.15</v>
+      </c>
+      <c r="B49" s="16">
+        <f t="shared" si="1"/>
+        <v>11.285539129341487</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="15">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B50" s="16">
+        <f t="shared" si="1"/>
+        <v>9.9039264769240276</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="15">
+        <v>2.25</v>
+      </c>
+      <c r="B51" s="16">
+        <f t="shared" si="1"/>
+        <v>8.5043478113066726</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="15">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B52" s="16">
+        <f t="shared" si="1"/>
+        <v>7.0830445637105299</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="15">
+        <v>2.35</v>
+      </c>
+      <c r="B53" s="16">
+        <f t="shared" si="1"/>
+        <v>5.6358533365022367</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="15">
+        <v>2.4</v>
+      </c>
+      <c r="B54" s="16">
+        <f t="shared" si="1"/>
+        <v>4.1581067262493434</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="15">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="B55" s="16">
+        <f t="shared" si="1"/>
+        <v>2.6445080777326098</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="B56" s="16">
+        <f t="shared" si="1"/>
+        <v>1.088970662157692</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="15">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="B57" s="16">
+        <f t="shared" si="1"/>
+        <v>-0.51559241654928201</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="15">
+        <v>2.6</v>
+      </c>
+      <c r="B58" s="16">
+        <f t="shared" si="1"/>
+        <v>-2.1775477564728476</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="15">
+        <v>2.65</v>
+      </c>
+      <c r="B59" s="16">
+        <f t="shared" si="1"/>
+        <v>-3.9069210617709587</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="15">
+        <v>2.7</v>
+      </c>
+      <c r="B60" s="16">
+        <f t="shared" si="1"/>
+        <v>-5.7159235818964476</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="15">
+        <v>2.75</v>
+      </c>
+      <c r="B61" s="16">
+        <f t="shared" si="1"/>
+        <v>-7.6197009771478861</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="15">
+        <v>2.8</v>
+      </c>
+      <c r="B62" s="16">
+        <f t="shared" si="1"/>
+        <v>-9.6374294493601838</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="15">
+        <v>2.85</v>
+      </c>
+      <c r="B63" s="16">
+        <f t="shared" si="1"/>
+        <v>-11.793974535950554</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="15">
+        <v>2.9</v>
+      </c>
+      <c r="B64" s="16">
+        <f t="shared" si="1"/>
+        <v>-14.122502737830132</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="15">
+        <v>2.95</v>
+      </c>
+      <c r="B65" s="16">
+        <f t="shared" si="1"/>
+        <v>-16.668795322814162</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="15">
+        <v>3</v>
+      </c>
+      <c r="B66" s="16">
+        <f t="shared" si="1"/>
+        <v>-19.498810814754705</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="15">
+        <v>3.05</v>
+      </c>
+      <c r="B67" s="16">
+        <f t="shared" si="1"/>
+        <v>-22.712991819120049</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="15">
+        <v>3.1</v>
+      </c>
+      <c r="B68" s="16">
+        <f t="shared" si="1"/>
+        <v>-26.476219372872094</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="15">
+        <v>3.15</v>
+      </c>
+      <c r="B69" s="16">
+        <f t="shared" si="1"/>
+        <v>-31.090168576091429</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="15">
+        <v>3.2</v>
+      </c>
+      <c r="B70" s="16">
+        <f t="shared" si="1"/>
+        <v>-37.211298628077486</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="17">
+        <v>3.25</v>
+      </c>
+      <c r="B71" s="18">
+        <f t="shared" ref="B71:B102" si="2">1/(1/$B$3 * LN((($B$4*A71)/($B$5-A71))/$B$2)+1/($B$1+273.15)) - 273.15</f>
+        <v>-46.839474542638158</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{255A40C7-1308-4ADA-AD9B-7D7D84E0AB57}">
+  <dimension ref="A1:AD24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" customWidth="1"/>
+    <col min="18" max="18" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="1.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="1.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.5703125" style="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="S1" s="2"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="12"/>
+      <c r="AD1" s="2"/>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1000</v>
+      </c>
+      <c r="B2">
+        <v>3.3</v>
+      </c>
+      <c r="C2" s="9">
+        <v>6299</v>
+      </c>
+      <c r="D2" s="10">
+        <f>($B$2*C2)/($A$2+C2)</f>
+        <v>2.8478832716810518</v>
+      </c>
+      <c r="E2" s="9">
+        <f>C2*($A$6+$A$7)/(C2+$A$6+$A$7)</f>
+        <v>2121.9917886093272</v>
+      </c>
+      <c r="F2" s="11">
+        <f>(($B$2*E2)/($B$6+E2))*$A$6/($A$6+$A$7)</f>
+        <v>1.5420504589321482</v>
+      </c>
+      <c r="G2" s="10">
+        <v>37.777777777777779</v>
+      </c>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T2" s="4">
+        <f>D2</f>
+        <v>2.8478832716810518</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="W2" s="12">
+        <f>G2</f>
+        <v>37.777777777777779</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z2" s="4">
+        <f>F2</f>
+        <v>1.5420504589321482</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC2" s="12">
+        <f>G2</f>
+        <v>37.777777777777779</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C3" s="9">
+        <v>4316</v>
+      </c>
+      <c r="D3" s="10">
+        <f t="shared" ref="D3:D11" si="0">($B$2*C3)/($A$2+C3)</f>
+        <v>2.6792325056433408</v>
+      </c>
+      <c r="E3" s="9">
+        <f t="shared" ref="E3:E12" si="1">C3*($A$6+$A$7)/(C3+$A$6+$A$7)</f>
+        <v>1837.5731772219265</v>
+      </c>
+      <c r="F3" s="11">
+        <f>(($B$2*E3)/($B$6+E3))*$A$6/($A$6+$A$7)</f>
+        <v>1.4692111482051089</v>
+      </c>
+      <c r="G3" s="10">
+        <v>48.888888888888886</v>
+      </c>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T3" s="4">
+        <f t="shared" ref="T3:T12" si="2">D3</f>
+        <v>2.6792325056433408</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="W3" s="12">
+        <f t="shared" ref="W3:W12" si="3">G3</f>
+        <v>48.888888888888886</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z3" s="4">
+        <f t="shared" ref="Z3:Z12" si="4">F3</f>
+        <v>1.4692111482051089</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC3" s="12">
+        <f t="shared" ref="AC3:AC12" si="5">G3</f>
+        <v>48.888888888888886</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="9">
+        <v>3020</v>
+      </c>
+      <c r="D4" s="10">
+        <f t="shared" si="0"/>
+        <v>2.4791044776119402</v>
+      </c>
+      <c r="E4" s="9">
+        <f t="shared" si="1"/>
+        <v>1553.6977491961416</v>
+      </c>
+      <c r="F4" s="11">
+        <f>(($B$2*E4)/($B$6+E4))*$A$6/($A$6+$A$7)</f>
+        <v>1.3803324099722991</v>
+      </c>
+      <c r="G4" s="10">
+        <v>60</v>
+      </c>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T4" s="4">
+        <f t="shared" si="2"/>
+        <v>2.4791044776119402</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="W4" s="12">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z4" s="4">
+        <f t="shared" si="4"/>
+        <v>1.3803324099722991</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC4" s="12">
+        <f t="shared" si="5"/>
+        <v>60</v>
+      </c>
+      <c r="AD4" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="9">
+        <v>2158</v>
+      </c>
+      <c r="D5" s="10">
+        <f>($B$2*C5)/($A$2+C5)</f>
+        <v>2.2550348321722606</v>
+      </c>
+      <c r="E5" s="9">
+        <f t="shared" si="1"/>
+        <v>1288.8391190742814</v>
+      </c>
+      <c r="F5" s="11">
+        <f>(($B$2*E5)/($B$6+E5))*$A$6/($A$6+$A$7)</f>
+        <v>1.2775269904432627</v>
+      </c>
+      <c r="G5" s="10">
+        <v>71.111111111111114</v>
+      </c>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T5" s="4">
+        <f t="shared" si="2"/>
+        <v>2.2550348321722606</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="W5" s="12">
+        <f t="shared" si="3"/>
+        <v>71.111111111111114</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z5" s="4">
+        <f t="shared" si="4"/>
+        <v>1.2775269904432627</v>
+      </c>
+      <c r="AA5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC5" s="12">
+        <f t="shared" si="5"/>
+        <v>71.111111111111114</v>
+      </c>
+      <c r="AD5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2200</v>
+      </c>
+      <c r="B6">
+        <v>1000</v>
+      </c>
+      <c r="C6" s="9">
+        <v>1569</v>
+      </c>
+      <c r="D6" s="10">
+        <f>($B$2*C6)/($A$2+C6)</f>
+        <v>2.0154534838458544</v>
+      </c>
+      <c r="E6" s="9">
+        <f t="shared" si="1"/>
+        <v>1052.7993289997903</v>
+      </c>
+      <c r="F6" s="11">
+        <f t="shared" ref="F6:F11" si="6">(($B$2*E6)/($B$6+E6))*$A$6/($A$6+$A$7)</f>
+        <v>1.1635518600992869</v>
+      </c>
+      <c r="G6" s="10">
+        <v>82.222222222222229</v>
+      </c>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T6" s="4">
+        <f t="shared" si="2"/>
+        <v>2.0154534838458544</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="W6" s="12">
+        <f t="shared" si="3"/>
+        <v>82.222222222222229</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z6" s="4">
+        <f t="shared" si="4"/>
+        <v>1.1635518600992869</v>
+      </c>
+      <c r="AA6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC6" s="12">
+        <f t="shared" si="5"/>
+        <v>82.222222222222229</v>
+      </c>
+      <c r="AD6" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1000</v>
+      </c>
+      <c r="C7" s="9">
+        <v>1160</v>
+      </c>
+      <c r="D7" s="10">
+        <f>($B$2*C7)/($A$2+C7)</f>
+        <v>1.7722222222222221</v>
+      </c>
+      <c r="E7" s="9">
+        <f t="shared" si="1"/>
+        <v>851.37614678899081</v>
+      </c>
+      <c r="F7" s="11">
+        <f>(($B$2*E7)/($B$6+E7))*$A$6/($A$6+$A$7)</f>
+        <v>1.0433102081268582</v>
+      </c>
+      <c r="G7" s="10">
+        <v>93.333333333333329</v>
+      </c>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T7" s="4">
+        <f t="shared" si="2"/>
+        <v>1.7722222222222221</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="W7" s="12">
+        <f t="shared" si="3"/>
+        <v>93.333333333333329</v>
+      </c>
+      <c r="X7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z7" s="4">
+        <f t="shared" si="4"/>
+        <v>1.0433102081268582</v>
+      </c>
+      <c r="AA7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC7" s="12">
+        <f t="shared" si="5"/>
+        <v>93.333333333333329</v>
+      </c>
+      <c r="AD7" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C8" s="9">
+        <v>870</v>
+      </c>
+      <c r="D8" s="10">
+        <f t="shared" si="0"/>
+        <v>1.5352941176470589</v>
+      </c>
+      <c r="E8" s="9">
+        <f t="shared" si="1"/>
+        <v>684.02948402948402</v>
+      </c>
+      <c r="F8" s="11">
+        <f>(($B$2*E8)/($B$6+E8))*$A$6/($A$6+$A$7)</f>
+        <v>0.92153487014881807</v>
+      </c>
+      <c r="G8" s="10">
+        <v>104.44444444444444</v>
+      </c>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T8" s="4">
+        <f t="shared" si="2"/>
+        <v>1.5352941176470589</v>
+      </c>
+      <c r="U8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="W8" s="12">
+        <f t="shared" si="3"/>
+        <v>104.44444444444444</v>
+      </c>
+      <c r="X8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z8" s="4">
+        <f t="shared" si="4"/>
+        <v>0.92153487014881807</v>
+      </c>
+      <c r="AA8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC8" s="12">
+        <f t="shared" si="5"/>
+        <v>104.44444444444444</v>
+      </c>
+      <c r="AD8" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C9" s="9">
+        <v>665</v>
+      </c>
+      <c r="D9" s="10">
+        <f t="shared" si="0"/>
+        <v>1.3180180180180181</v>
+      </c>
+      <c r="E9" s="9">
+        <f t="shared" si="1"/>
+        <v>550.58214747736088</v>
+      </c>
+      <c r="F9" s="11">
+        <f t="shared" si="6"/>
+        <v>0.80558985483063561</v>
+      </c>
+      <c r="G9" s="10">
+        <v>115.55555555555556</v>
+      </c>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T9" s="4">
+        <f t="shared" si="2"/>
+        <v>1.3180180180180181</v>
+      </c>
+      <c r="U9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="W9" s="12">
+        <f t="shared" si="3"/>
+        <v>115.55555555555556</v>
+      </c>
+      <c r="X9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z9" s="4">
+        <f t="shared" si="4"/>
+        <v>0.80558985483063561</v>
+      </c>
+      <c r="AA9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC9" s="12">
+        <f t="shared" si="5"/>
+        <v>115.55555555555556</v>
+      </c>
+      <c r="AD9" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C10" s="9">
+        <v>515</v>
+      </c>
+      <c r="D10" s="10">
+        <f t="shared" si="0"/>
+        <v>1.1217821782178219</v>
+      </c>
+      <c r="E10" s="9">
+        <f t="shared" si="1"/>
+        <v>443.60699865410498</v>
+      </c>
+      <c r="F10" s="11">
+        <f t="shared" si="6"/>
+        <v>0.69716576542979669</v>
+      </c>
+      <c r="G10" s="10">
+        <v>126.66666666666667</v>
+      </c>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T10" s="4">
+        <f t="shared" si="2"/>
+        <v>1.1217821782178219</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="W10" s="12">
+        <f t="shared" si="3"/>
+        <v>126.66666666666667</v>
+      </c>
+      <c r="X10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z10" s="4">
+        <f t="shared" si="4"/>
+        <v>0.69716576542979669</v>
+      </c>
+      <c r="AA10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC10" s="12">
+        <f t="shared" si="5"/>
+        <v>126.66666666666667</v>
+      </c>
+      <c r="AD10" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C11" s="9">
+        <v>405</v>
+      </c>
+      <c r="D11" s="10">
+        <f t="shared" si="0"/>
+        <v>0.95124555160142343</v>
+      </c>
+      <c r="E11" s="9">
+        <f t="shared" si="1"/>
+        <v>359.50069348127602</v>
+      </c>
+      <c r="F11" s="11">
+        <f t="shared" si="6"/>
+        <v>0.5999387880024486</v>
+      </c>
+      <c r="G11" s="10">
+        <v>137.77777777777777</v>
+      </c>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T11" s="4">
+        <f t="shared" si="2"/>
+        <v>0.95124555160142343</v>
+      </c>
+      <c r="U11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="W11" s="12">
+        <f t="shared" si="3"/>
+        <v>137.77777777777777</v>
+      </c>
+      <c r="X11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z11" s="4">
+        <f t="shared" si="4"/>
+        <v>0.5999387880024486</v>
+      </c>
+      <c r="AA11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC11" s="12">
+        <f t="shared" si="5"/>
+        <v>137.77777777777777</v>
+      </c>
+      <c r="AD11" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C12" s="9">
+        <v>323</v>
+      </c>
+      <c r="D12" s="10">
+        <f>($B$2*C12)/($A$2+C12)</f>
+        <v>0.80566893424036268</v>
+      </c>
+      <c r="E12" s="9">
+        <f t="shared" si="1"/>
+        <v>293.38631847856942</v>
+      </c>
+      <c r="F12" s="11">
+        <f>(($B$2*E12)/($B$6+E12))*$A$6/($A$6+$A$7)</f>
+        <v>0.51463371812316205</v>
+      </c>
+      <c r="G12" s="10">
+        <v>148.88888888888889</v>
+      </c>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T12" s="4">
+        <f t="shared" si="2"/>
+        <v>0.80566893424036268</v>
+      </c>
+      <c r="U12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="W12" s="12">
+        <f t="shared" si="3"/>
+        <v>148.88888888888889</v>
+      </c>
+      <c r="X12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z12" s="4">
+        <f t="shared" si="4"/>
+        <v>0.51463371812316205</v>
+      </c>
+      <c r="AA12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC12" s="12">
+        <f t="shared" si="5"/>
+        <v>148.88888888888889</v>
+      </c>
+      <c r="AD12" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="S13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="T13" s="4"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="12"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z13" s="4"/>
+      <c r="AA13" s="2"/>
+      <c r="AB13" s="2"/>
+      <c r="AC13" s="12"/>
+      <c r="AD13" s="2"/>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C14" s="9"/>
+      <c r="G14" s="9"/>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C15" s="9"/>
+      <c r="G15" s="9"/>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C16" s="9"/>
+      <c r="G16" s="9"/>
+    </row>
+    <row r="19" spans="13:26" x14ac:dyDescent="0.25">
+      <c r="M19" s="5"/>
+    </row>
+    <row r="22" spans="13:26" x14ac:dyDescent="0.25">
+      <c r="M22" s="1"/>
+    </row>
+    <row r="24" spans="13:26" x14ac:dyDescent="0.25">
+      <c r="T24"/>
+      <c r="Z24"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -27330,7 +31517,7 @@
   <dimension ref="A1:AD45"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="D2" sqref="D2:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>